<commit_message>
file path url updated
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Method Name</t>
   </si>
@@ -23,25 +23,13 @@
     <t>Execution Data</t>
   </si>
   <si>
-    <t>verifyCustomerNavigationToRegistrationPage</t>
+    <t>test</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>27-10-2024</t>
-  </si>
-  <si>
-    <t>verifyNewCustomerRegistrationSubmissionFlow</t>
-  </si>
-  <si>
-    <t>verifyCustomerRegistrationAndLoginNavigation</t>
-  </si>
-  <si>
-    <t>verifyCustomerEmailActivation</t>
-  </si>
-  <si>
-    <t>verifyCustomerSuccessfulLogin</t>
+    <t>29-10-2024</t>
   </si>
 </sst>
 </file>
@@ -88,12 +76,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
@@ -101,13 +85,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="44.0390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.046875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>
@@ -134,50 +118,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
log file save method updated
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Method Name</t>
   </si>
@@ -23,13 +23,25 @@
     <t>Execution Data</t>
   </si>
   <si>
-    <t>test</t>
+    <t>verifyCustomerNavigationToRegistrationPage</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
     <t>29-10-2024</t>
+  </si>
+  <si>
+    <t>verifyNewCustomerRegistrationSubmissionFlow</t>
+  </si>
+  <si>
+    <t>verifyCustomerRegistrationAndLoginNavigation</t>
+  </si>
+  <si>
+    <t>verifyCustomerEmailActivation</t>
+  </si>
+  <si>
+    <t>verifyCustomerSuccessfulLogin</t>
   </si>
 </sst>
 </file>
@@ -76,8 +88,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
@@ -85,13 +101,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="44.0390625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>
@@ -118,6 +134,50 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added subscription selection page
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Method Name</t>
   </si>
@@ -23,25 +23,19 @@
     <t>Execution Data</t>
   </si>
   <si>
-    <t>verifyCustomerNavigationToRegistrationPage</t>
+    <t>verifyCustomerSuccessfulLogin</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>29-10-2024</t>
+    <t>03-11-2024</t>
   </si>
   <si>
-    <t>verifyNewCustomerRegistrationSubmissionFlow</t>
+    <t>verifyCustomerPreferredPackageSelection</t>
   </si>
   <si>
-    <t>verifyCustomerRegistrationAndLoginNavigation</t>
-  </si>
-  <si>
-    <t>verifyCustomerEmailActivation</t>
-  </si>
-  <si>
-    <t>verifyCustomerSuccessfulLogin</t>
+    <t>verifyCustomerNavigationAfterSaving</t>
   </si>
 </sst>
 </file>
@@ -88,10 +82,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -101,13 +93,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="44.0390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.81640625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>
@@ -156,28 +148,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
added contact info page
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Method Name</t>
   </si>
@@ -29,13 +29,16 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>03-11-2024</t>
+    <t>04-11-2024</t>
   </si>
   <si>
     <t>verifyCustomerPreferredPackageSelection</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterSaving</t>
+  </si>
+  <si>
+    <t>verifyCustomerBasicInfoEntry</t>
   </si>
 </sst>
 </file>
@@ -82,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -93,7 +97,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -148,6 +152,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
contact info page added
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>Method Name</t>
   </si>
@@ -23,13 +23,28 @@
     <t>Execution Data</t>
   </si>
   <si>
+    <t>verifyCustomerNavigationToRegistrationPage</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>10-11-2024</t>
+  </si>
+  <si>
+    <t>verifyNewCustomerRegistrationSubmissionFlow</t>
+  </si>
+  <si>
+    <t>verifyCustomerRegistrationAndLoginNavigation</t>
+  </si>
+  <si>
+    <t>verifyCustomerEmailActivation</t>
+  </si>
+  <si>
     <t>verifyCustomerSuccessfulLogin</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>04-11-2024</t>
+    <t>verifyCustomerNavigationAfterLogin</t>
   </si>
   <si>
     <t>verifyCustomerPreferredPackageSelection</t>
@@ -85,8 +100,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -97,13 +118,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="38.81640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="44.0390625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>
@@ -163,6 +184,72 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s" s="9">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
location and user page added
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>Method Name</t>
   </si>
@@ -44,9 +44,6 @@
     <t>verifyCustomerSuccessfulLogin</t>
   </si>
   <si>
-    <t>verifyCustomerNavigationAfterLogin</t>
-  </si>
-  <si>
     <t>verifyCustomerPreferredPackageSelection</t>
   </si>
   <si>
@@ -54,6 +51,12 @@
   </si>
   <si>
     <t>verifyCustomerBasicInfoEntry</t>
+  </si>
+  <si>
+    <t>verifyCustomerStoreInfoEntry</t>
+  </si>
+  <si>
+    <t>verifyCustomerLicenseInfoEntry</t>
   </si>
 </sst>
 </file>
@@ -100,8 +103,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -118,7 +123,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -230,7 +235,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s" s="9">
         <v>4</v>
@@ -241,12 +246,34 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s" s="10">
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s" s="11">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s" s="12">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
validation added on license page
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Method Name</t>
   </si>
@@ -29,13 +29,10 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>14-11-2024</t>
+    <t>24-11-2024</t>
   </si>
   <si>
-    <t>verifyCustomerCreditCardInfoAndSubmitOrder</t>
-  </si>
-  <si>
-    <t>verifyCustomerNavigationAfterPayment</t>
+    <t>verifyCustomerLicenseInfoEntry</t>
   </si>
 </sst>
 </file>
@@ -82,9 +79,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
@@ -93,13 +89,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.04296875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="29.609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>
@@ -137,17 +133,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
start paid subscription completed
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Method Name</t>
   </si>
@@ -29,19 +29,16 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>01-12-2024</t>
+    <t>02-12-2024</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterLogin</t>
   </si>
   <si>
-    <t>verifyStartPaidSubscriptionManually</t>
+    <t>verifyCustomerNewSeasonalLicensePurchase</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterPayment</t>
-  </si>
-  <si>
-    <t>verifyProratedPaymentDetails</t>
   </si>
   <si>
     <t>verifyCustomerReceiptPageWithProratedOrderDetails</t>
@@ -94,9 +91,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -109,7 +105,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -197,17 +193,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
code refactor and update
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -29,13 +29,13 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>02-12-2024</t>
+    <t>05-12-2024</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterLogin</t>
   </si>
   <si>
-    <t>verifyCustomerNewSeasonalLicensePurchase</t>
+    <t>verifyCustomerAdditionalLicensePurchase</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterPayment</t>
@@ -44,7 +44,7 @@
     <t>verifyCustomerReceiptPageWithProratedOrderDetails</t>
   </si>
   <si>
-    <t>verifyCustomerReceivedSeasonalLicenseReceipt</t>
+    <t>verifyCustomerReceivedSubscriptionUpgradeReceipt</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
test case 9 added
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -35,7 +35,7 @@
     <t>verifyCustomerNavigationAfterLogin</t>
   </si>
   <si>
-    <t>verifyCustomerPackageUpgradeAndSeasonalPurchase</t>
+    <t>verifyCustomerPackageDowngradeAndLicensePurchase</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterPayment</t>
@@ -111,7 +111,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.11328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="50.73046875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>

<commit_message>
test case 12 added
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -35,16 +35,16 @@
     <t>verifyCustomerNavigationAfterLogin</t>
   </si>
   <si>
-    <t>verifyCustomerPackageUpgradeAndLicensePurchase</t>
+    <t>verifyCustomerPackageAndLicenseDowngrade</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterPayment</t>
   </si>
   <si>
-    <t>verifyCustomerReceiptPageWithProratedAndRecurringOrderDetails</t>
+    <t>verifyCustomerReceiptPageWithRecurringOrderDetails</t>
   </si>
   <si>
-    <t>verifyCustomerReceivedSubscriptionUpgradeReceipt</t>
+    <t>verifyCustomerReceivedSubscriptionDowngradeReceipt</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="61.5703125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="50.9921875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>

<commit_message>
test case 13 added
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -29,22 +29,22 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>17-12-2024</t>
+    <t>18-12-2024</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterLogin</t>
   </si>
   <si>
-    <t>verifyCustomerPackageAndLicenseDowngrade</t>
+    <t>verifyCustomerPackageUpgradeAndLicensePurchase</t>
   </si>
   <si>
     <t>verifyCustomerNavigationAfterPayment</t>
   </si>
   <si>
-    <t>verifyCustomerReceiptPageWithRecurringOrderDetails</t>
+    <t>verifyCustomerReceiptPageWithProratedAndRecurringOrderDetails</t>
   </si>
   <si>
-    <t>verifyCustomerReceivedSubscriptionDowngradeReceipt</t>
+    <t>verifyCustomerReceivedSubscriptionUpgradeReceipt</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.9921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="61.5703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>

<commit_message>
value type settings page added
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Method Name</t>
   </si>
@@ -29,16 +29,13 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>27-12-2024</t>
+    <t>28-12-2024</t>
   </si>
   <si>
     <t>verifyHomeMenuVisibilityAfterLogin</t>
   </si>
   <si>
-    <t>verifyCustomerNavigationAfterLogin</t>
-  </si>
-  <si>
-    <t>verifyTipsCategoryValueListAddition</t>
+    <t>verifyValueTypeSettingMap</t>
   </si>
 </sst>
 </file>
@@ -85,12 +82,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -100,13 +93,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="33.71484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.58203125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>
@@ -155,50 +148,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s" s="6">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
customer maintenance page added
</commit_message>
<xml_diff>
--- a/Test Results/Test_Result.xlsx
+++ b/Test Results/Test_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Method Name</t>
   </si>
@@ -35,7 +35,13 @@
     <t>verifyHomeMenuVisibilityAfterLogin</t>
   </si>
   <si>
-    <t>verifyValueTypeSettingMap</t>
+    <t>verifyCustomerNavigationAfterLogin</t>
+  </si>
+  <si>
+    <t>verifyCustomerDataEntry</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -52,7 +58,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -67,6 +73,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -82,24 +98,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="33.58203125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.71484375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.85546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.5" customWidth="true" bestFit="true"/>
   </cols>
@@ -148,6 +170,72 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>